<commit_message>
modified:   Enter/Catapult/README.md 	modified:   Jack/README.md 	modified:   Zomboni/README.md 	modified:   Zomboni/zomboni_test_info.xlsx
</commit_message>
<xml_diff>
--- a/Zomboni/zomboni_test_info.xlsx
+++ b/Zomboni/zomboni_test_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="12975"/>
+    <workbookView windowWidth="27750" windowHeight="10665"/>
   </bookViews>
   <sheets>
     <sheet name="守一" sheetId="9" r:id="rId1"/>
@@ -89,7 +89,7 @@
     <t>是</t>
   </si>
   <si>
-    <t>锁植物反应</t>
+    <t>锁植物攻击间隔</t>
   </si>
   <si>
     <t>随机</t>
@@ -285,6 +285,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -363,12 +375,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -406,12 +412,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -602,7 +602,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -626,16 +626,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -644,60 +644,60 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -726,7 +726,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -746,6 +746,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1276,7 +1282,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -1356,7 +1362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="4:15">
+    <row r="3" s="1" customFormat="1" spans="1:15">
       <c r="D3" s="6">
         <v>7</v>
       </c>
@@ -1447,10 +1453,10 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6">
@@ -1510,7 +1516,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="4:15">
+    <row r="8" s="1" customFormat="1" spans="1:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1528,7 +1534,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:15">
+    <row r="9" s="1" customFormat="1" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1540,7 +1546,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="4:15">
+    <row r="10" s="1" customFormat="1" spans="1:15">
       <c r="D10" s="6">
         <v>6</v>
       </c>
@@ -1566,7 +1572,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="4:15">
+    <row r="11" s="1" customFormat="1" spans="1:15">
       <c r="D11" s="6">
         <v>5</v>
       </c>
@@ -1592,7 +1598,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:15">
+    <row r="12" s="1" customFormat="1" spans="1:15">
       <c r="D12" s="6">
         <v>4</v>
       </c>
@@ -1618,7 +1624,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="4:15">
+    <row r="13" s="1" customFormat="1" spans="1:15">
       <c r="D13" s="6">
         <v>3</v>
       </c>
@@ -1644,7 +1650,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="4:15">
+    <row r="14" s="1" customFormat="1" spans="1:15">
       <c r="D14" s="6">
         <v>2</v>
       </c>
@@ -1670,7 +1676,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="4:15">
+    <row r="15" s="1" customFormat="1" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1688,7 +1694,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="4:15">
+    <row r="16" s="1" customFormat="1" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -1858,7 +1864,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -1938,7 +1944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="4:15">
+    <row r="3" s="1" customFormat="1" spans="1:15">
       <c r="D3" s="6">
         <v>7</v>
       </c>
@@ -2029,10 +2035,10 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6">
@@ -2092,7 +2098,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="4:15">
+    <row r="8" s="1" customFormat="1" spans="1:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2110,7 +2116,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:15">
+    <row r="9" s="1" customFormat="1" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2122,7 +2128,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="4:15">
+    <row r="10" s="1" customFormat="1" spans="1:15">
       <c r="D10" s="6">
         <v>6</v>
       </c>
@@ -2148,7 +2154,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="4:15">
+    <row r="11" s="1" customFormat="1" spans="1:15">
       <c r="D11" s="6">
         <v>5</v>
       </c>
@@ -2174,7 +2180,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:15">
+    <row r="12" s="1" customFormat="1" spans="1:15">
       <c r="D12" s="6">
         <v>4</v>
       </c>
@@ -2200,7 +2206,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="4:15">
+    <row r="13" s="1" customFormat="1" spans="1:15">
       <c r="D13" s="6">
         <v>3</v>
       </c>
@@ -2226,7 +2232,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="4:15">
+    <row r="14" s="1" customFormat="1" spans="1:15">
       <c r="D14" s="6">
         <v>2</v>
       </c>
@@ -2252,7 +2258,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="4:15">
+    <row r="15" s="1" customFormat="1" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -2270,7 +2276,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="4:15">
+    <row r="16" s="1" customFormat="1" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -2441,7 +2447,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -2521,7 +2527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="4:15">
+    <row r="3" s="1" customFormat="1" spans="1:15">
       <c r="D3" s="6">
         <v>7</v>
       </c>
@@ -2612,10 +2618,10 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6">
@@ -2675,7 +2681,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="4:15">
+    <row r="8" s="1" customFormat="1" spans="1:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2693,7 +2699,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:15">
+    <row r="9" s="1" customFormat="1" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2705,7 +2711,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="4:15">
+    <row r="10" s="1" customFormat="1" spans="1:15">
       <c r="D10" s="6">
         <v>6</v>
       </c>
@@ -2731,7 +2737,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="4:15">
+    <row r="11" s="1" customFormat="1" spans="1:15">
       <c r="D11" s="6">
         <v>5</v>
       </c>
@@ -2757,7 +2763,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:15">
+    <row r="12" s="1" customFormat="1" spans="1:15">
       <c r="D12" s="6">
         <v>4</v>
       </c>
@@ -2783,7 +2789,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="4:15">
+    <row r="13" s="1" customFormat="1" spans="1:15">
       <c r="D13" s="6">
         <v>3</v>
       </c>
@@ -2809,7 +2815,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="4:15">
+    <row r="14" s="1" customFormat="1" spans="1:15">
       <c r="D14" s="6">
         <v>2</v>
       </c>
@@ -2835,7 +2841,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="4:15">
+    <row r="15" s="1" customFormat="1" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -2853,7 +2859,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="4:15">
+    <row r="16" s="1" customFormat="1" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -3024,7 +3030,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -3104,7 +3110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="4:15">
+    <row r="3" spans="1:15">
       <c r="D3" s="6">
         <v>7</v>
       </c>
@@ -3195,10 +3201,10 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6">
@@ -3258,7 +3264,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="4:15">
+    <row r="8" spans="1:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -3276,7 +3282,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="4:15">
+    <row r="9" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -3288,7 +3294,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="4:15">
+    <row r="10" spans="1:15">
       <c r="D10" s="6">
         <v>6</v>
       </c>
@@ -3314,7 +3320,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="4:15">
+    <row r="11" spans="1:15">
       <c r="D11" s="6">
         <v>5</v>
       </c>
@@ -3340,7 +3346,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="4:15">
+    <row r="12" spans="1:15">
       <c r="D12" s="6">
         <v>4</v>
       </c>
@@ -3366,7 +3372,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="4:15">
+    <row r="13" spans="1:15">
       <c r="D13" s="6">
         <v>3</v>
       </c>
@@ -3392,7 +3398,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="4:15">
+    <row r="14" spans="1:15">
       <c r="D14" s="6">
         <v>2</v>
       </c>
@@ -3418,7 +3424,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="4:15">
+    <row r="15" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -3436,7 +3442,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="4:15">
+    <row r="16" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -3607,7 +3613,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="168" zoomScaleNormal="168" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -3686,7 +3692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="4:15">
+    <row r="3" s="1" customFormat="1" spans="1:15">
       <c r="D3" s="6">
         <v>9</v>
       </c>
@@ -3777,10 +3783,10 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6">
@@ -3832,7 +3838,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="4:15">
+    <row r="8" s="1" customFormat="1" spans="1:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -3850,7 +3856,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:15">
+    <row r="9" s="1" customFormat="1" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -3862,7 +3868,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="4:15">
+    <row r="10" s="1" customFormat="1" spans="1:15">
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -3880,7 +3886,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="4:15">
+    <row r="11" s="1" customFormat="1" spans="1:15">
       <c r="D11" s="6">
         <v>7</v>
       </c>
@@ -3906,7 +3912,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:15">
+    <row r="12" s="1" customFormat="1" spans="1:15">
       <c r="D12" s="6">
         <v>6</v>
       </c>
@@ -3932,7 +3938,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="4:15">
+    <row r="13" s="1" customFormat="1" spans="1:15">
       <c r="D13" s="6">
         <v>5</v>
       </c>
@@ -3958,7 +3964,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="4:15">
+    <row r="14" s="1" customFormat="1" spans="1:15">
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -3976,7 +3982,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="4:15">
+    <row r="15" s="1" customFormat="1" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -3994,7 +4000,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="4:15">
+    <row r="16" s="1" customFormat="1" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -4158,7 +4164,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -4237,7 +4243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="4:15">
+    <row r="3" s="1" customFormat="1" spans="1:15">
       <c r="D3" s="6">
         <v>9</v>
       </c>
@@ -4328,10 +4334,10 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6">
@@ -4391,7 +4397,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="4:15">
+    <row r="8" s="1" customFormat="1" spans="1:15">
       <c r="D8" s="6">
         <v>5</v>
       </c>
@@ -4417,7 +4423,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:15">
+    <row r="9" s="1" customFormat="1" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -4429,7 +4435,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="4:15">
+    <row r="10" s="1" customFormat="1" spans="1:15">
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -4447,7 +4453,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="4:15">
+    <row r="11" s="1" customFormat="1" spans="1:15">
       <c r="D11" s="6">
         <v>6</v>
       </c>
@@ -4473,7 +4479,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:15">
+    <row r="12" s="1" customFormat="1" spans="1:15">
       <c r="D12" s="6">
         <v>5</v>
       </c>
@@ -4499,7 +4505,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="4:15">
+    <row r="13" s="1" customFormat="1" spans="1:15">
       <c r="D13" s="6">
         <v>4</v>
       </c>
@@ -4525,7 +4531,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="4:15">
+    <row r="14" s="1" customFormat="1" spans="1:15">
       <c r="D14" s="6">
         <v>3</v>
       </c>
@@ -4551,7 +4557,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="4:15">
+    <row r="15" s="1" customFormat="1" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -4569,7 +4575,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="4:15">
+    <row r="16" s="1" customFormat="1" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -4733,7 +4739,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
@@ -4812,7 +4818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="4:15">
+    <row r="3" s="1" customFormat="1" spans="1:15">
       <c r="D3" s="6">
         <v>5</v>
       </c>
@@ -4903,10 +4909,10 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:15">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="6">
@@ -4966,7 +4972,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="4:15">
+    <row r="8" s="1" customFormat="1" spans="1:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -4984,7 +4990,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="4:15">
+    <row r="9" s="1" customFormat="1" spans="1:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -4996,7 +5002,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="4:15">
+    <row r="10" s="1" customFormat="1" spans="1:15">
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -5014,7 +5020,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="4:15">
+    <row r="11" s="1" customFormat="1" spans="1:15">
       <c r="D11" s="6">
         <v>4</v>
       </c>
@@ -5040,7 +5046,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="4:15">
+    <row r="12" s="1" customFormat="1" spans="1:15">
       <c r="D12" s="6">
         <v>3</v>
       </c>
@@ -5066,7 +5072,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="4:15">
+    <row r="13" s="1" customFormat="1" spans="1:15">
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -5092,7 +5098,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="4:15">
+    <row r="14" s="1" customFormat="1" spans="1:15">
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -5104,7 +5110,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="4:15">
+    <row r="15" s="1" customFormat="1" spans="1:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -5116,7 +5122,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="4:15">
+    <row r="16" s="1" customFormat="1" spans="1:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>

</xml_diff>

<commit_message>
新测试 	modified:   .gitignore 	modified:   Zomboni/zomboni_config.json 	modified:   Zomboni/zomboni_test_info.xlsx 	modified:   output.csv 	modified:   test.cpp
</commit_message>
<xml_diff>
--- a/Zomboni/zomboni_test_info.xlsx
+++ b/Zomboni/zomboni_test_info.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="27750" windowHeight="10665"/>
+    <workbookView windowHeight="15100"/>
   </bookViews>
   <sheets>
-    <sheet name="tmp" sheetId="4" r:id="rId1"/>
-    <sheet name="守一" sheetId="9" r:id="rId2"/>
-    <sheet name="守五" sheetId="8" r:id="rId3"/>
-    <sheet name="守六" sheetId="1" r:id="rId4"/>
+    <sheet name="守六" sheetId="1" r:id="rId1"/>
+    <sheet name="tmp" sheetId="4" r:id="rId2"/>
+    <sheet name="守一" sheetId="9" r:id="rId3"/>
+    <sheet name="守五" sheetId="8" r:id="rId4"/>
     <sheet name="守八" sheetId="2" r:id="rId5"/>
     <sheet name="守七" sheetId="7" r:id="rId6"/>
     <sheet name="守四" sheetId="6" r:id="rId7"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="22">
   <si>
     <t>被压列数</t>
   </si>
@@ -74,9 +74,6 @@
     <t>曾</t>
   </si>
   <si>
-    <t>非永动</t>
-  </si>
-  <si>
     <t>永动</t>
   </si>
   <si>
@@ -89,19 +86,19 @@
     <t>是</t>
   </si>
   <si>
+    <t>非永动</t>
+  </si>
+  <si>
     <t>锁植物攻击间隔</t>
   </si>
   <si>
-    <t>最慢</t>
+    <t>随机</t>
   </si>
   <si>
     <t>时间上限</t>
   </si>
   <si>
     <t>喷</t>
-  </si>
-  <si>
-    <t>随机</t>
   </si>
 </sst>
 </file>
@@ -1281,34 +1278,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet8"/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.69166666666667" style="1"/>
-    <col min="3" max="3" width="9.23333333333333" style="1"/>
-    <col min="4" max="7" width="9.23333333333333" style="2"/>
-    <col min="8" max="8" width="9.23333333333333" style="1"/>
-    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23333333333333" style="2"/>
-    <col min="12" max="12" width="9.23333333333333" style="1"/>
-    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23333333333333" style="2"/>
-    <col min="16" max="16384" width="9.23333333333333" style="1"/>
+    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.69230769230769" style="1"/>
+    <col min="3" max="3" width="9.23076923076923" style="1"/>
+    <col min="4" max="7" width="9.23076923076923" style="2"/>
+    <col min="8" max="8" width="9.23076923076923" style="1"/>
+    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23076923076923" style="2"/>
+    <col min="12" max="12" width="9.23076923076923" style="1"/>
+    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23076923076923" style="2"/>
+    <col min="16" max="16384" width="9.23076923076923" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:15">
+    <row r="1" spans="1:15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1327,7 +1324,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:15">
+    <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1365,9 +1362,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:15">
+    <row r="3" spans="4:15">
       <c r="D3" s="6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>12</v>
@@ -1376,24 +1373,24 @@
         <v>13</v>
       </c>
       <c r="G3" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="4">
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K3" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" s="1" customFormat="1" spans="1:15">
+    <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4">
         <v>1000000</v>
@@ -1405,16 +1402,16 @@
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4" s="4">
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" s="6">
         <v>0</v>
@@ -1423,12 +1420,12 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" s="1" customFormat="1" spans="1:15">
+    <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="6">
         <v>5</v>
@@ -1437,16 +1434,16 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G5" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="4">
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -1455,7 +1452,7 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:15">
+    <row r="6" spans="1:15">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
@@ -1469,7 +1466,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -1478,7 +1475,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -1487,7 +1484,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:15">
+    <row r="7" spans="1:15">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1501,7 +1498,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -1510,7 +1507,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -1519,7 +1516,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="1:15">
+    <row r="8" spans="4:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1528,7 +1525,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -1537,7 +1534,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="1:15">
+    <row r="9" spans="4:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1549,7 +1546,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="1:15">
+    <row r="10" spans="4:15">
       <c r="D10" s="6">
         <v>6</v>
       </c>
@@ -1557,7 +1554,7 @@
         <v>21</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="6">
         <v>0</v>
@@ -1566,7 +1563,7 @@
         <v>0.875</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K10" s="6">
         <v>0</v>
@@ -1575,7 +1572,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:15">
+    <row r="11" spans="4:15">
       <c r="D11" s="6">
         <v>5</v>
       </c>
@@ -1583,7 +1580,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="6">
         <v>0</v>
@@ -1592,7 +1589,7 @@
         <v>1.375</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
@@ -1601,7 +1598,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:15">
+    <row r="12" spans="4:15">
       <c r="D12" s="6">
         <v>4</v>
       </c>
@@ -1609,16 +1606,16 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="4">
         <v>1.375</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K12" s="6">
         <v>0</v>
@@ -1627,7 +1624,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:15">
+    <row r="13" spans="4:15">
       <c r="D13" s="6">
         <v>3</v>
       </c>
@@ -1635,7 +1632,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -1644,7 +1641,7 @@
         <v>1.1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K13" s="6">
         <v>0</v>
@@ -1653,7 +1650,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="1:15">
+    <row r="14" spans="4:15">
       <c r="D14" s="6">
         <v>2</v>
       </c>
@@ -1661,7 +1658,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -1670,7 +1667,7 @@
         <v>0.8125</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K14" s="6">
         <v>0</v>
@@ -1679,7 +1676,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="1:15">
+    <row r="15" spans="4:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1688,7 +1685,7 @@
         <v>0.525</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K15" s="6">
         <v>0</v>
@@ -1697,7 +1694,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:15">
+    <row r="16" spans="4:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -1709,7 +1706,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" s="1" customFormat="1" spans="4:15">
+    <row r="17" spans="4:15">
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -1718,7 +1715,7 @@
         <v>0.1</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K17" s="6">
         <v>0</v>
@@ -1727,7 +1724,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" s="1" customFormat="1" spans="4:15">
+    <row r="18" spans="4:15">
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -1737,7 +1734,7 @@
         <v>-0.1875</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K18" s="6">
         <v>0</v>
@@ -1746,7 +1743,7 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" s="1" customFormat="1" spans="4:15">
+    <row r="19" spans="4:15">
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -1758,7 +1755,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" s="1" customFormat="1" spans="4:15">
+    <row r="20" spans="4:15">
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -1770,7 +1767,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" s="1" customFormat="1" spans="4:15">
+    <row r="21" spans="4:15">
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -1782,7 +1779,7 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" s="1" customFormat="1" spans="4:15">
+    <row r="22" spans="4:15">
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -1794,7 +1791,7 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" s="1" customFormat="1" spans="4:15">
+    <row r="23" spans="4:15">
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -1806,7 +1803,7 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" s="1" customFormat="1" spans="4:15">
+    <row r="24" spans="4:15">
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -1818,7 +1815,7 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
     </row>
-    <row r="25" s="1" customFormat="1" spans="4:15">
+    <row r="25" spans="4:15">
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -1867,26 +1864,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.69166666666667" style="1"/>
-    <col min="3" max="3" width="9.23333333333333" style="1"/>
-    <col min="4" max="7" width="9.23333333333333" style="2"/>
-    <col min="8" max="8" width="9.23333333333333" style="1"/>
-    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23333333333333" style="2"/>
-    <col min="12" max="12" width="9.23333333333333" style="1"/>
-    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23333333333333" style="2"/>
-    <col min="16" max="16384" width="9.23333333333333" style="1"/>
+    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.69230769230769" style="1"/>
+    <col min="3" max="3" width="9.23076923076923" style="1"/>
+    <col min="4" max="7" width="9.23076923076923" style="2"/>
+    <col min="8" max="8" width="9.23076923076923" style="1"/>
+    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23076923076923" style="2"/>
+    <col min="12" max="12" width="9.23076923076923" style="1"/>
+    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23076923076923" style="2"/>
+    <col min="16" max="16384" width="9.23076923076923" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:15">
@@ -1894,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1951,7 +1948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:15">
+    <row r="3" s="1" customFormat="1" spans="4:15">
       <c r="D3" s="6">
         <v>7</v>
       </c>
@@ -1959,7 +1956,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
@@ -1968,10 +1965,10 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K3" s="6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -1979,13 +1976,13 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4">
         <v>1000000</v>
       </c>
       <c r="D4" s="6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
@@ -1994,16 +1991,16 @@
         <v>13</v>
       </c>
       <c r="G4" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="4">
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
@@ -2011,13 +2008,13 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:15">
       <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>12</v>
@@ -2026,13 +2023,13 @@
         <v>13</v>
       </c>
       <c r="G5" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5" s="4">
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -2046,7 +2043,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6">
         <v>5</v>
@@ -2055,7 +2052,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -2064,7 +2061,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -2087,7 +2084,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -2096,7 +2093,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -2105,7 +2102,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="1:15">
+    <row r="8" s="1" customFormat="1" spans="4:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2114,7 +2111,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -2123,7 +2120,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="1:15">
+    <row r="9" s="1" customFormat="1" spans="4:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2135,7 +2132,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="1:15">
+    <row r="10" s="1" customFormat="1" spans="4:15">
       <c r="D10" s="6">
         <v>6</v>
       </c>
@@ -2143,7 +2140,7 @@
         <v>21</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="6">
         <v>0</v>
@@ -2152,7 +2149,7 @@
         <v>0.875</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K10" s="6">
         <v>0</v>
@@ -2161,7 +2158,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:15">
+    <row r="11" s="1" customFormat="1" spans="4:15">
       <c r="D11" s="6">
         <v>5</v>
       </c>
@@ -2169,16 +2166,16 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="4">
         <v>1.375</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
@@ -2187,7 +2184,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:15">
+    <row r="12" s="1" customFormat="1" spans="4:15">
       <c r="D12" s="6">
         <v>4</v>
       </c>
@@ -2195,7 +2192,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="6">
         <v>0</v>
@@ -2204,7 +2201,7 @@
         <v>1.375</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K12" s="6">
         <v>0</v>
@@ -2213,7 +2210,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:15">
+    <row r="13" s="1" customFormat="1" spans="4:15">
       <c r="D13" s="6">
         <v>3</v>
       </c>
@@ -2221,7 +2218,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -2230,7 +2227,7 @@
         <v>1.1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K13" s="6">
         <v>0</v>
@@ -2239,7 +2236,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="1:15">
+    <row r="14" s="1" customFormat="1" spans="4:15">
       <c r="D14" s="6">
         <v>2</v>
       </c>
@@ -2247,7 +2244,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -2256,7 +2253,7 @@
         <v>0.8125</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K14" s="6">
         <v>0</v>
@@ -2265,7 +2262,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="1:15">
+    <row r="15" s="1" customFormat="1" spans="4:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -2274,7 +2271,7 @@
         <v>0.525</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K15" s="6">
         <v>0</v>
@@ -2283,7 +2280,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:15">
+    <row r="16" s="1" customFormat="1" spans="4:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -2304,7 +2301,7 @@
         <v>0.1</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K17" s="6">
         <v>0</v>
@@ -2323,592 +2320,7 @@
         <v>-0.1875</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="6">
-        <v>0</v>
-      </c>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-    </row>
-    <row r="19" s="1" customFormat="1" spans="4:15">
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-    </row>
-    <row r="20" s="1" customFormat="1" spans="4:15">
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-    </row>
-    <row r="21" s="1" customFormat="1" spans="4:15">
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-    </row>
-    <row r="22" s="1" customFormat="1" spans="4:15">
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-    </row>
-    <row r="23" s="1" customFormat="1" spans="4:15">
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-    </row>
-    <row r="24" s="1" customFormat="1" spans="4:15">
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-    </row>
-    <row r="25" s="1" customFormat="1" spans="4:15">
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-  </mergeCells>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"普通,南瓜,冰道,炮"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
-      <formula1>"是,否"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"随机,最快,最慢"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D25">
-      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
-      <formula1>"曾,喷"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25 J3:J25 N3:N25">
-      <formula1>"永动,非永动"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:O25"/>
-  <sheetViews>
-    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.69166666666667" style="1"/>
-    <col min="3" max="3" width="9.23333333333333" style="1"/>
-    <col min="4" max="7" width="9.23333333333333" style="2"/>
-    <col min="8" max="8" width="9.23333333333333" style="1"/>
-    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23333333333333" style="2"/>
-    <col min="12" max="12" width="9.23333333333333" style="1"/>
-    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23333333333333" style="2"/>
-    <col min="16" max="16384" width="9.23333333333333" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:15">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4">
-        <v>5</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="I1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="M1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:15">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" s="1" customFormat="1" spans="1:15">
-      <c r="D3" s="6">
-        <v>7</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="6">
-        <v>0</v>
-      </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-    </row>
-    <row r="4" s="1" customFormat="1" spans="1:15">
-      <c r="A4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1000000</v>
-      </c>
-      <c r="D4" s="6">
-        <v>8</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" s="1" customFormat="1" spans="1:15">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="6">
-        <v>5</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:15">
-      <c r="A6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="6">
-        <v>5</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:15">
-      <c r="A7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="3">
-        <v>3500</v>
-      </c>
-      <c r="D7" s="6">
-        <v>8</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4">
-        <v>1.25</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="6">
-        <v>0</v>
-      </c>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:15">
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="I8" s="4">
-        <v>2</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="6">
-        <v>0</v>
-      </c>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:15">
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="1:15">
-      <c r="D10" s="6">
-        <v>6</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0</v>
-      </c>
-      <c r="I10" s="4">
-        <v>0.875</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="1:15">
-      <c r="D11" s="6">
-        <v>5</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="I11" s="4">
-        <v>1.375</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="1:15">
-      <c r="D12" s="6">
-        <v>4</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="I12" s="4">
-        <v>1.375</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="6">
-        <v>0</v>
-      </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:15">
-      <c r="D13" s="6">
-        <v>3</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0</v>
-      </c>
-      <c r="I13" s="4">
-        <v>1.1</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="6">
-        <v>0</v>
-      </c>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-    </row>
-    <row r="14" s="1" customFormat="1" spans="1:15">
-      <c r="D14" s="6">
-        <v>2</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0.8125</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="6">
-        <v>0</v>
-      </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-    </row>
-    <row r="15" s="1" customFormat="1" spans="1:15">
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="I15" s="4">
-        <v>0.525</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="6">
-        <v>0</v>
-      </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:15">
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="4:15">
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="I17" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" s="6">
-        <v>0</v>
-      </c>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" s="1" customFormat="1" spans="4:15">
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="I18" s="4">
-        <f>0.8125-1</f>
-        <v>-0.1875</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K18" s="6">
         <v>0</v>
@@ -3036,36 +2448,36 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.69166666666667" style="1"/>
-    <col min="3" max="3" width="9.23333333333333" style="1"/>
-    <col min="4" max="7" width="9.23333333333333" style="2"/>
-    <col min="8" max="8" width="9.23333333333333" style="1"/>
-    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23333333333333" style="2"/>
-    <col min="12" max="12" width="9.23333333333333" style="1"/>
-    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23333333333333" style="2"/>
-    <col min="16" max="16384" width="9.23333333333333" style="1"/>
+    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.69230769230769" style="1"/>
+    <col min="3" max="3" width="9.23076923076923" style="1"/>
+    <col min="4" max="7" width="9.23076923076923" style="2"/>
+    <col min="8" max="8" width="9.23076923076923" style="1"/>
+    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23076923076923" style="2"/>
+    <col min="12" max="12" width="9.23076923076923" style="1"/>
+    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23076923076923" style="2"/>
+    <col min="16" max="16384" width="9.23076923076923" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" s="1" customFormat="1" spans="1:15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -3084,7 +2496,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" s="1" customFormat="1" spans="1:15">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -3122,7 +2534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" s="1" customFormat="1" spans="4:15">
       <c r="D3" s="6">
         <v>7</v>
       </c>
@@ -3130,7 +2542,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
@@ -3139,39 +2551,39 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K3" s="6">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" s="1" customFormat="1" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4">
         <v>1000000</v>
       </c>
       <c r="D4" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G4" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4" s="4">
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" s="6">
         <v>0</v>
@@ -3180,30 +2592,30 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" s="1" customFormat="1" spans="1:15">
       <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="D5" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G5" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="4">
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -3212,12 +2624,12 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" s="1" customFormat="1" spans="1:15">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6">
         <v>5</v>
@@ -3226,7 +2638,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -3235,7 +2647,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -3244,7 +2656,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" s="1" customFormat="1" spans="1:15">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -3258,7 +2670,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -3267,7 +2679,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -3276,7 +2688,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" s="1" customFormat="1" spans="4:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -3285,7 +2697,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -3294,7 +2706,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" s="1" customFormat="1" spans="4:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -3306,7 +2718,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" s="1" customFormat="1" spans="4:15">
       <c r="D10" s="6">
         <v>6</v>
       </c>
@@ -3314,7 +2726,7 @@
         <v>21</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="6">
         <v>0</v>
@@ -3323,7 +2735,7 @@
         <v>0.875</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K10" s="6">
         <v>0</v>
@@ -3332,7 +2744,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" s="1" customFormat="1" spans="4:15">
       <c r="D11" s="6">
         <v>5</v>
       </c>
@@ -3340,7 +2752,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="6">
         <v>0</v>
@@ -3349,7 +2761,7 @@
         <v>1.375</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
@@ -3358,7 +2770,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" s="1" customFormat="1" spans="4:15">
       <c r="D12" s="6">
         <v>4</v>
       </c>
@@ -3366,7 +2778,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="6">
         <v>0</v>
@@ -3375,7 +2787,7 @@
         <v>1.375</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K12" s="6">
         <v>0</v>
@@ -3384,7 +2796,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" s="1" customFormat="1" spans="4:15">
       <c r="D13" s="6">
         <v>3</v>
       </c>
@@ -3392,7 +2804,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -3401,7 +2813,7 @@
         <v>1.1</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K13" s="6">
         <v>0</v>
@@ -3410,7 +2822,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" s="1" customFormat="1" spans="4:15">
       <c r="D14" s="6">
         <v>2</v>
       </c>
@@ -3418,7 +2830,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -3427,7 +2839,7 @@
         <v>0.8125</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K14" s="6">
         <v>0</v>
@@ -3436,7 +2848,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" s="1" customFormat="1" spans="4:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -3445,7 +2857,7 @@
         <v>0.525</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K15" s="6">
         <v>0</v>
@@ -3454,7 +2866,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" s="1" customFormat="1" spans="4:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -3466,7 +2878,7 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
-    <row r="17" spans="4:15">
+    <row r="17" s="1" customFormat="1" spans="4:15">
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -3475,7 +2887,7 @@
         <v>0.1</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K17" s="6">
         <v>0</v>
@@ -3484,7 +2896,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
     </row>
-    <row r="18" spans="4:15">
+    <row r="18" s="1" customFormat="1" spans="4:15">
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -3494,7 +2906,7 @@
         <v>-0.1875</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K18" s="6">
         <v>0</v>
@@ -3503,7 +2915,7 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="4:15">
+    <row r="19" s="1" customFormat="1" spans="4:15">
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -3515,7 +2927,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
     </row>
-    <row r="20" spans="4:15">
+    <row r="20" s="1" customFormat="1" spans="4:15">
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -3527,7 +2939,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
     </row>
-    <row r="21" spans="4:15">
+    <row r="21" s="1" customFormat="1" spans="4:15">
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -3539,7 +2951,7 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
     </row>
-    <row r="22" spans="4:15">
+    <row r="22" s="1" customFormat="1" spans="4:15">
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -3551,7 +2963,7 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
     </row>
-    <row r="23" spans="4:15">
+    <row r="23" s="1" customFormat="1" spans="4:15">
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -3563,7 +2975,7 @@
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="4:15">
+    <row r="24" s="1" customFormat="1" spans="4:15">
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -3575,7 +2987,592 @@
       <c r="N24" s="5"/>
       <c r="O24" s="5"/>
     </row>
-    <row r="25" spans="4:15">
+    <row r="25" s="1" customFormat="1" spans="4:15">
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
+  </mergeCells>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"普通,南瓜,冰道,炮"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+      <formula1>"是,否"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"随机,最快,最慢"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D25">
+      <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E25">
+      <formula1>"曾,喷"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F25 J3:J25 N3:N25">
+      <formula1>"永动,非永动"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:O25"/>
+  <sheetViews>
+    <sheetView zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
+  <cols>
+    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.69230769230769" style="1"/>
+    <col min="3" max="3" width="9.23076923076923" style="1"/>
+    <col min="4" max="7" width="9.23076923076923" style="2"/>
+    <col min="8" max="8" width="9.23076923076923" style="1"/>
+    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23076923076923" style="2"/>
+    <col min="12" max="12" width="9.23076923076923" style="1"/>
+    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23076923076923" style="2"/>
+    <col min="16" max="16384" width="9.23076923076923" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:15">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="M1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:15">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="4:15">
+      <c r="D3" s="6">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:15">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1000000</v>
+      </c>
+      <c r="D4" s="6">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:15">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:15">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:15">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3500</v>
+      </c>
+      <c r="D7" s="6">
+        <v>8</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="4:15">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="I8" s="4">
+        <v>2</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="4:15">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="4:15">
+      <c r="D10" s="6">
+        <v>6</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.875</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="4:15">
+      <c r="D11" s="6">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1.375</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="4:15">
+      <c r="D12" s="6">
+        <v>4</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1.375</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="4:15">
+      <c r="D13" s="6">
+        <v>3</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1.1</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="4:15">
+      <c r="D14" s="6">
+        <v>2</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0.8125</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0</v>
+      </c>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="4:15">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="I15" s="4">
+        <v>0.525</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="6">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="4:15">
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="4:15">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="I17" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="4:15">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="I18" s="4">
+        <f>0.8125-1</f>
+        <v>-0.1875</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0</v>
+      </c>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="4:15">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="4:15">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="4:15">
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="4:15">
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="4:15">
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="4:15">
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="4:15">
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -3631,18 +3628,18 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23333333333333" style="1"/>
-    <col min="4" max="7" width="9.23333333333333" style="2"/>
-    <col min="8" max="8" width="9.23333333333333" style="1"/>
-    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23333333333333" style="2"/>
-    <col min="12" max="12" width="9.23333333333333" style="1"/>
-    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23333333333333" style="2"/>
-    <col min="16" max="16384" width="9.23333333333333" style="1"/>
+    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.23076923076923" style="1"/>
+    <col min="4" max="7" width="9.23076923076923" style="2"/>
+    <col min="8" max="8" width="9.23076923076923" style="1"/>
+    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23076923076923" style="2"/>
+    <col min="12" max="12" width="9.23076923076923" style="1"/>
+    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23076923076923" style="2"/>
+    <col min="16" max="16384" width="9.23076923076923" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:15">
@@ -3707,7 +3704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:15">
+    <row r="3" s="1" customFormat="1" spans="4:15">
       <c r="D3" s="6">
         <v>9</v>
       </c>
@@ -3715,7 +3712,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>
@@ -3724,7 +3721,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K3" s="6">
         <v>0</v>
@@ -3735,7 +3732,7 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4">
         <v>10000</v>
@@ -3747,7 +3744,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="6">
         <v>3</v>
@@ -3756,7 +3753,7 @@
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" s="6">
         <v>9</v>
@@ -3767,10 +3764,10 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:15">
       <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="6">
         <v>7</v>
@@ -3779,7 +3776,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="6">
         <v>1</v>
@@ -3788,7 +3785,7 @@
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -3802,7 +3799,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6">
         <v>7</v>
@@ -3811,7 +3808,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G6" s="6">
         <v>1</v>
@@ -3820,7 +3817,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -3844,7 +3841,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -3853,7 +3850,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="1:15">
+    <row r="8" s="1" customFormat="1" spans="4:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -3862,7 +3859,7 @@
         <v>1.5</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -3871,7 +3868,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="1:15">
+    <row r="9" s="1" customFormat="1" spans="4:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -3883,7 +3880,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="1:15">
+    <row r="10" s="1" customFormat="1" spans="4:15">
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -3892,7 +3889,7 @@
         <v>2.1</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K10" s="6">
         <v>1</v>
@@ -3901,7 +3898,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:15">
+    <row r="11" s="1" customFormat="1" spans="4:15">
       <c r="D11" s="6">
         <v>7</v>
       </c>
@@ -3909,7 +3906,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="6">
         <v>1</v>
@@ -3918,7 +3915,7 @@
         <v>1.95</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K11" s="6">
         <v>1</v>
@@ -3927,7 +3924,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:15">
+    <row r="12" s="1" customFormat="1" spans="4:15">
       <c r="D12" s="6">
         <v>6</v>
       </c>
@@ -3935,7 +3932,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="6">
         <v>1</v>
@@ -3944,7 +3941,7 @@
         <v>1.6625</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K12" s="6">
         <v>1</v>
@@ -3953,7 +3950,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:15">
+    <row r="13" s="1" customFormat="1" spans="4:15">
       <c r="D13" s="6">
         <v>5</v>
       </c>
@@ -3961,7 +3958,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -3970,7 +3967,7 @@
         <v>1.375</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K13" s="6">
         <v>2</v>
@@ -3979,7 +3976,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="1:15">
+    <row r="14" s="1" customFormat="1" spans="4:15">
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -3988,7 +3985,7 @@
         <v>1.1</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K14" s="6">
         <v>1</v>
@@ -3997,7 +3994,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="1:15">
+    <row r="15" s="1" customFormat="1" spans="4:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -4006,7 +4003,7 @@
         <v>0.8125</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K15" s="6">
         <v>0</v>
@@ -4015,7 +4012,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:15">
+    <row r="16" s="1" customFormat="1" spans="4:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -4024,7 +4021,7 @@
         <v>0.525</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K16" s="6">
         <v>0</v>
@@ -4185,18 +4182,18 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23333333333333" style="1"/>
-    <col min="4" max="7" width="9.23333333333333" style="2"/>
-    <col min="8" max="8" width="9.23333333333333" style="1"/>
-    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23333333333333" style="2"/>
-    <col min="12" max="12" width="9.23333333333333" style="1"/>
-    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23333333333333" style="2"/>
-    <col min="16" max="16384" width="9.23333333333333" style="1"/>
+    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.23076923076923" style="1"/>
+    <col min="4" max="7" width="9.23076923076923" style="2"/>
+    <col min="8" max="8" width="9.23076923076923" style="1"/>
+    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23076923076923" style="2"/>
+    <col min="12" max="12" width="9.23076923076923" style="1"/>
+    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23076923076923" style="2"/>
+    <col min="16" max="16384" width="9.23076923076923" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:15">
@@ -4261,7 +4258,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:15">
+    <row r="3" s="1" customFormat="1" spans="4:15">
       <c r="D3" s="6">
         <v>9</v>
       </c>
@@ -4269,7 +4266,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
@@ -4278,7 +4275,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K3" s="6">
         <v>13</v>
@@ -4289,7 +4286,7 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4">
         <v>100000</v>
@@ -4301,7 +4298,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="6">
         <v>0</v>
@@ -4310,7 +4307,7 @@
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" s="6">
         <v>0</v>
@@ -4321,10 +4318,10 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:15">
       <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="6">
         <v>7</v>
@@ -4333,7 +4330,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" s="6">
         <v>3</v>
@@ -4342,7 +4339,7 @@
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -4356,7 +4353,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6">
         <v>6</v>
@@ -4365,7 +4362,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -4374,7 +4371,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -4397,7 +4394,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -4406,7 +4403,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -4415,7 +4412,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="1:15">
+    <row r="8" s="1" customFormat="1" spans="4:15">
       <c r="D8" s="6">
         <v>5</v>
       </c>
@@ -4423,7 +4420,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" s="6">
         <v>0</v>
@@ -4432,7 +4429,7 @@
         <v>1.5</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -4441,7 +4438,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="1:15">
+    <row r="9" s="1" customFormat="1" spans="4:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -4453,7 +4450,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="1:15">
+    <row r="10" s="1" customFormat="1" spans="4:15">
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -4462,7 +4459,7 @@
         <v>2.1</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K10" s="6">
         <v>0</v>
@@ -4471,7 +4468,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:15">
+    <row r="11" s="1" customFormat="1" spans="4:15">
       <c r="D11" s="6">
         <v>6</v>
       </c>
@@ -4479,7 +4476,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="6">
         <v>0</v>
@@ -4488,7 +4485,7 @@
         <v>1.95</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
@@ -4497,7 +4494,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:15">
+    <row r="12" s="1" customFormat="1" spans="4:15">
       <c r="D12" s="6">
         <v>5</v>
       </c>
@@ -4505,7 +4502,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="6">
         <v>0</v>
@@ -4514,7 +4511,7 @@
         <v>1.6625</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K12" s="6">
         <v>0</v>
@@ -4523,7 +4520,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:15">
+    <row r="13" s="1" customFormat="1" spans="4:15">
       <c r="D13" s="6">
         <v>4</v>
       </c>
@@ -4531,7 +4528,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -4540,7 +4537,7 @@
         <v>1.375</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K13" s="6">
         <v>0</v>
@@ -4549,7 +4546,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="1:15">
+    <row r="14" s="1" customFormat="1" spans="4:15">
       <c r="D14" s="6">
         <v>3</v>
       </c>
@@ -4557,7 +4554,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -4566,7 +4563,7 @@
         <v>1.1</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K14" s="6">
         <v>0</v>
@@ -4575,7 +4572,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="1:15">
+    <row r="15" s="1" customFormat="1" spans="4:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -4584,7 +4581,7 @@
         <v>0.8125</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K15" s="6">
         <v>0</v>
@@ -4593,7 +4590,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:15">
+    <row r="16" s="1" customFormat="1" spans="4:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -4602,7 +4599,7 @@
         <v>0.525</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K16" s="6">
         <v>0</v>
@@ -4763,18 +4760,18 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23333333333333" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="17.3666666666667" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.23333333333333" style="1"/>
-    <col min="4" max="7" width="9.23333333333333" style="2"/>
-    <col min="8" max="8" width="9.23333333333333" style="1"/>
-    <col min="9" max="9" width="10.0083333333333" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23333333333333" style="2"/>
-    <col min="12" max="12" width="9.23333333333333" style="1"/>
-    <col min="13" max="13" width="10.8666666666667" style="2" customWidth="1"/>
-    <col min="14" max="15" width="9.23333333333333" style="2"/>
-    <col min="16" max="16384" width="9.23333333333333" style="1"/>
+    <col min="1" max="1" width="17.3653846153846" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.23076923076923" style="1"/>
+    <col min="4" max="7" width="9.23076923076923" style="2"/>
+    <col min="8" max="8" width="9.23076923076923" style="1"/>
+    <col min="9" max="9" width="10.0096153846154" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.23076923076923" style="2"/>
+    <col min="12" max="12" width="9.23076923076923" style="1"/>
+    <col min="13" max="13" width="10.8653846153846" style="2" customWidth="1"/>
+    <col min="14" max="15" width="9.23076923076923" style="2"/>
+    <col min="16" max="16384" width="9.23076923076923" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:15">
@@ -4839,7 +4836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:15">
+    <row r="3" s="1" customFormat="1" spans="4:15">
       <c r="D3" s="6">
         <v>5</v>
       </c>
@@ -4847,7 +4844,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>
@@ -4856,7 +4853,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K3" s="6">
         <v>0</v>
@@ -4867,7 +4864,7 @@
     </row>
     <row r="4" s="1" customFormat="1" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4">
         <v>10000</v>
@@ -4879,7 +4876,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="6">
         <v>0</v>
@@ -4888,7 +4885,7 @@
         <v>0.5</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" s="6">
         <v>0</v>
@@ -4899,10 +4896,10 @@
     </row>
     <row r="5" s="1" customFormat="1" spans="1:15">
       <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="6">
         <v>4</v>
@@ -4911,7 +4908,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G5" s="6">
         <v>0</v>
@@ -4920,7 +4917,7 @@
         <v>0.25</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5" s="6">
         <v>0</v>
@@ -4934,7 +4931,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="6">
         <v>3</v>
@@ -4943,7 +4940,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -4952,7 +4949,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="6">
         <v>0</v>
@@ -4975,7 +4972,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -4984,7 +4981,7 @@
         <v>1.25</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7" s="6">
         <v>0</v>
@@ -4993,7 +4990,7 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" s="1" customFormat="1" spans="1:15">
+    <row r="8" s="1" customFormat="1" spans="4:15">
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -5002,7 +4999,7 @@
         <v>1.5</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K8" s="6">
         <v>0</v>
@@ -5011,7 +5008,7 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
-    <row r="9" s="1" customFormat="1" spans="1:15">
+    <row r="9" s="1" customFormat="1" spans="4:15">
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -5023,7 +5020,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
     </row>
-    <row r="10" s="1" customFormat="1" spans="1:15">
+    <row r="10" s="1" customFormat="1" spans="4:15">
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -5032,7 +5029,7 @@
         <v>1.375</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K10" s="6">
         <v>4</v>
@@ -5041,7 +5038,7 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:15">
+    <row r="11" s="1" customFormat="1" spans="4:15">
       <c r="D11" s="6">
         <v>4</v>
       </c>
@@ -5049,7 +5046,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="6">
         <v>1</v>
@@ -5058,7 +5055,7 @@
         <v>1.1</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K11" s="6">
         <v>0</v>
@@ -5067,7 +5064,7 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:15">
+    <row r="12" s="1" customFormat="1" spans="4:15">
       <c r="D12" s="6">
         <v>3</v>
       </c>
@@ -5075,7 +5072,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="6">
         <v>0</v>
@@ -5084,7 +5081,7 @@
         <v>0.8125</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K12" s="6">
         <v>0</v>
@@ -5093,7 +5090,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:15">
+    <row r="13" s="1" customFormat="1" spans="4:15">
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -5101,7 +5098,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -5110,7 +5107,7 @@
         <v>0.525</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K13" s="6">
         <v>0</v>
@@ -5119,7 +5116,7 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" s="1" customFormat="1" spans="1:15">
+    <row r="14" s="1" customFormat="1" spans="4:15">
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -5131,7 +5128,7 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
-    <row r="15" s="1" customFormat="1" spans="1:15">
+    <row r="15" s="1" customFormat="1" spans="4:15">
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -5143,7 +5140,7 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:15">
+    <row r="16" s="1" customFormat="1" spans="4:15">
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>

</xml_diff>